<commit_message>
Ended project with a relogin system
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -461,7 +461,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>399.5</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3">
@@ -491,7 +491,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>600.5</v>
+        <v>200.5</v>
       </c>
     </row>
     <row r="5">
@@ -521,7 +521,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7">

</xml_diff>